<commit_message>
added ingest and cal sheets for 327_D00002 (glider 327 telemetered data deployment 00002) and changed 326 cal sheet deployment time.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL326/Omaha_Cal_Info_CE05MOAS-GL326_00002.xlsx
+++ b/CE05MOAS-GL326/Omaha_Cal_Info_CE05MOAS-GL326_00002.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12390" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="12705" yWindow="-15" windowWidth="12510" windowHeight="12390" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +846,7 @@
         <v>42292</v>
       </c>
       <c r="E2" s="11">
-        <v>0.8208333333333333</v>
+        <v>0.79722222222222217</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="17" t="s">
@@ -883,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
recovered glider 326. added recovered ingest sheet and updated cal info with recovered date.
</commit_message>
<xml_diff>
--- a/CE05MOAS-GL326/Omaha_Cal_Info_CE05MOAS-GL326_00002.xlsx
+++ b/CE05MOAS-GL326/Omaha_Cal_Info_CE05MOAS-GL326_00002.xlsx
@@ -35,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$78</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$276</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -779,7 +779,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +848,9 @@
       <c r="E2" s="11">
         <v>0.79722222222222217</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="26">
+        <v>42318</v>
+      </c>
       <c r="G2" s="17" t="s">
         <v>31</v>
       </c>

</xml_diff>